<commit_message>
fix: fix pages margins
</commit_message>
<xml_diff>
--- a/act.xlsx
+++ b/act.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\xistore_repair-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D95CF27-2ADC-49A0-8527-93B1FF8AF2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4082ECF-FB85-4E1A-ACF7-595AB191EB6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2805" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="квитанция" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Приемщик:</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Заказчик </t>
   </si>
   <si>
-    <t>Савицкий А.С.</t>
-  </si>
-  <si>
     <t>1. Диагностика и ремонт осуществляются в срок до 30 дней (п. 1 ст. 22 Закона "О защите прав потребителей") со дня передачи устройства для целей диагностики и определения возможности проведения ремонтных работ.</t>
   </si>
   <si>
@@ -172,36 +169,6 @@
   </si>
   <si>
     <t>Подменный фонд:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Гарантийный ремонт; </t>
-  </si>
-  <si>
-    <t>Свыше 30 дней</t>
-  </si>
-  <si>
-    <t>Внешний аккумулятор Redmi Power Bank 20000 мАч (белый с кабелем)</t>
-  </si>
-  <si>
-    <t>24983/00105145</t>
-  </si>
-  <si>
-    <t>Состояние б/у, царапины и потертости на корпусе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Аппарат, Коробка, Гарантийный талон, Кабель, </t>
-  </si>
-  <si>
-    <t>26.08.2020</t>
-  </si>
-  <si>
-    <t>Не заряжается и не заряжает другие устройства</t>
-  </si>
-  <si>
-    <t>ООО Ньюстэйдж (Магазин "Xistore", г. Могилев Планета Green)</t>
-  </si>
-  <si>
-    <t>Старовойтова Инна Анатольевна</t>
   </si>
 </sst>
 </file>
@@ -360,10 +327,11 @@
       <charset val="204"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -804,9 +772,93 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -819,9 +871,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,72 +880,12 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -904,27 +893,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1363,8 +1331,8 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,27 +1345,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
+      <c r="B2" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1410,20 +1378,20 @@
       <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="31" t="str">
+      <c r="C5" s="31">
         <f>B53</f>
-        <v>Савицкий А.С.</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="29">
         <f ca="1">NOW()</f>
-        <v>44180.92952002315</v>
+        <v>44180.944622800926</v>
       </c>
       <c r="D6" s="27"/>
     </row>
@@ -1441,117 +1409,101 @@
     </row>
     <row r="9" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="51" t="str">
+      <c r="B9" s="53" t="str">
         <f ca="1">"КВИТАНЦИЯ " &amp; DAY(TODAY()) &amp; "/" &amp; MONTH(TODAY()) &amp; "/20"</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
     </row>
     <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
     </row>
     <row r="11" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="57"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="63"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="51"/>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="1" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="63"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="B17" s="46"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
+        <v>26</v>
+      </c>
+      <c r="B18" s="42"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="71"/>
-    </row>
-    <row r="20" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
+        <v>45</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="75"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
@@ -1560,23 +1512,23 @@
     </row>
     <row r="22" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="A23" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
@@ -1584,7 +1536,7 @@
     </row>
     <row r="25" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
@@ -1592,7 +1544,7 @@
     </row>
     <row r="26" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -1600,7 +1552,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="34"/>
       <c r="C27" s="34"/>
@@ -1608,7 +1560,7 @@
     </row>
     <row r="28" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -1616,7 +1568,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
@@ -1624,7 +1576,7 @@
     </row>
     <row r="30" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -1632,7 +1584,7 @@
     </row>
     <row r="31" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -1640,7 +1592,7 @@
     </row>
     <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="34"/>
       <c r="C32" s="34"/>
@@ -1648,7 +1600,7 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="34"/>
       <c r="C33" s="34"/>
@@ -1656,23 +1608,23 @@
     </row>
     <row r="34" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="34"/>
       <c r="C34" s="34"/>
       <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
+      <c r="A35" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="34"/>
       <c r="C36" s="34"/>
@@ -1680,7 +1632,7 @@
     </row>
     <row r="37" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
@@ -1696,40 +1648,37 @@
       <c r="A39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="35"/>
+      <c r="C39" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="str">
-        <f>B55</f>
-        <v>Старовойтова Инна Анатольевна</v>
-      </c>
+      <c r="A41" s="32"/>
       <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="72" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="72"/>
+      <c r="C42" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="36"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="35"/>
+      <c r="D43" s="37"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
@@ -1744,10 +1693,7 @@
       <c r="D45" s="13"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="str">
-        <f>B53</f>
-        <v>Савицкий А.С.</v>
-      </c>
+      <c r="A46" s="20"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
       <c r="D46" s="13"/>
@@ -1768,7 +1714,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
     </row>
@@ -1783,140 +1729,110 @@
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25">
         <f ca="1">C6</f>
-        <v>44180.92952002315</v>
-      </c>
-      <c r="B51" s="75" t="str">
+        <v>44180.944622800926</v>
+      </c>
+      <c r="B51" s="45" t="str">
         <f ca="1">B9</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C51" s="75"/>
+      <c r="C51" s="45"/>
       <c r="D51" s="24"/>
     </row>
     <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="40" t="str">
-        <f>B12</f>
-        <v>Внешний аккумулятор Redmi Power Bank 20000 мАч (белый с кабелем)</v>
-      </c>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
+      <c r="B52" s="57"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="69"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="45"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="45"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="40"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="45"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="48">
-        <v>80298199591</v>
-      </c>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="72"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="48" t="str">
-        <f>B13</f>
-        <v>24983/00105145</v>
-      </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="72"/>
     </row>
     <row r="58" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="47" t="str">
-        <f>B14</f>
-        <v>Состояние б/у, царапины и потертости на корпусе</v>
-      </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="45"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="47" t="str">
-        <f>B16</f>
-        <v xml:space="preserve">Аппарат, Коробка, Гарантийный талон, Кабель, </v>
-      </c>
-      <c r="C59" s="44"/>
-      <c r="D59" s="45"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="47" t="str">
-        <f>B15</f>
-        <v xml:space="preserve">Гарантийный ремонт; </v>
-      </c>
-      <c r="C60" s="44"/>
-      <c r="D60" s="45"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B61" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="45"/>
+        <v>27</v>
+      </c>
+      <c r="B61" s="52"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" s="73"/>
-      <c r="D62" s="74"/>
+        <v>26</v>
+      </c>
+      <c r="B62" s="42"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="44"/>
     </row>
     <row r="63" spans="1:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="37" t="str">
-        <f>B19</f>
-        <v>Не заряжается и не заряжает другие устройства</v>
-      </c>
-      <c r="C63" s="38"/>
-      <c r="D63" s="39"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="67"/>
     </row>
     <row r="64" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
@@ -1929,23 +1845,23 @@
     </row>
     <row r="66" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="34"/>
       <c r="C66" s="34"/>
       <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
+      <c r="A67" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B68" s="34"/>
       <c r="C68" s="34"/>
@@ -1953,7 +1869,7 @@
     </row>
     <row r="69" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" s="34"/>
       <c r="C69" s="34"/>
@@ -1961,7 +1877,7 @@
     </row>
     <row r="70" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B70" s="34"/>
       <c r="C70" s="34"/>
@@ -1969,7 +1885,7 @@
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B71" s="34"/>
       <c r="C71" s="34"/>
@@ -1977,7 +1893,7 @@
     </row>
     <row r="72" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B72" s="34"/>
       <c r="C72" s="34"/>
@@ -1985,7 +1901,7 @@
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B73" s="34"/>
       <c r="C73" s="34"/>
@@ -1993,7 +1909,7 @@
     </row>
     <row r="74" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" s="34"/>
       <c r="C74" s="34"/>
@@ -2001,7 +1917,7 @@
     </row>
     <row r="75" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B75" s="34"/>
       <c r="C75" s="34"/>
@@ -2009,7 +1925,7 @@
     </row>
     <row r="76" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B76" s="34"/>
       <c r="C76" s="34"/>
@@ -2017,7 +1933,7 @@
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B77" s="34"/>
       <c r="C77" s="34"/>
@@ -2025,23 +1941,23 @@
     </row>
     <row r="78" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B78" s="34"/>
       <c r="C78" s="34"/>
       <c r="D78" s="34"/>
     </row>
     <row r="79" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="B79" s="61"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
+      <c r="A79" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
     </row>
     <row r="80" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B80" s="34"/>
       <c r="C80" s="34"/>
@@ -2049,7 +1965,7 @@
     </row>
     <row r="81" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B81" s="34"/>
       <c r="C81" s="34"/>
@@ -2065,10 +1981,10 @@
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D83" s="35"/>
+      <c r="C83" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
@@ -2079,21 +1995,18 @@
       <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="str">
-        <f>B55</f>
-        <v>Старовойтова Инна Анатольевна</v>
-      </c>
+      <c r="A86" s="6"/>
       <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="36" t="str">
+      <c r="C87" s="64" t="str">
         <f>C42</f>
         <v>________________________________________ Дата_______________</v>
       </c>
-      <c r="D87" s="36"/>
+      <c r="D87" s="64"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
@@ -2115,10 +2028,7 @@
       <c r="C90" s="4"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="18" t="str">
-        <f>B53</f>
-        <v>Савицкий А.С.</v>
-      </c>
+      <c r="A91" s="18"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
     </row>
@@ -2156,31 +2066,30 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
@@ -2197,30 +2106,31 @@
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A70:D70"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A73:D73"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: add some changes in act
</commit_message>
<xml_diff>
--- a/act.xlsx
+++ b/act.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\xistore_repair-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4082ECF-FB85-4E1A-ACF7-595AB191EB6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70246C82-E5BF-47E7-B658-3692CD6705B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +334,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -754,9 +762,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -772,30 +777,117 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -805,95 +897,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1331,8 +1339,8 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,27 +1353,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1378,7 +1386,7 @@
       <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <f>B53</f>
         <v>0</v>
       </c>
@@ -1389,9 +1397,9 @@
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="75">
         <f ca="1">NOW()</f>
-        <v>44180.944622800926</v>
+        <v>44180.947744791665</v>
       </c>
       <c r="D6" s="27"/>
     </row>
@@ -1409,58 +1417,58 @@
     </row>
     <row r="9" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="53" t="str">
+      <c r="B9" s="50" t="str">
         <f ca="1">"КВИТАНЦИЯ " &amp; DAY(TODAY()) &amp; "/" &amp; MONTH(TODAY()) &amp; "/20"</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
     </row>
     <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
     </row>
     <row r="11" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="57"/>
-      <c r="D12" s="58"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="54"/>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="56"/>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="51"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="62"/>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="51"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="62"/>
       <c r="E15" t="s">
         <v>24</v>
       </c>
@@ -1469,174 +1477,174 @@
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="62"/>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="44"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="75"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="66"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
     </row>
     <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
     </row>
     <row r="34" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
     </row>
     <row r="35" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
     </row>
     <row r="36" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
     </row>
     <row r="37" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
@@ -1648,37 +1656,37 @@
       <c r="A39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="37"/>
+      <c r="D39" s="34"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="32"/>
+      <c r="A41" s="31"/>
       <c r="D41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="36"/>
+      <c r="D42" s="70"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="37"/>
+      <c r="D43" s="34"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
@@ -1714,7 +1722,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
     </row>
@@ -1729,247 +1737,247 @@
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25">
         <f ca="1">C6</f>
-        <v>44180.944622800926</v>
-      </c>
-      <c r="B51" s="45" t="str">
+        <v>44180.947744791665</v>
+      </c>
+      <c r="B51" s="73" t="str">
         <f ca="1">B9</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C51" s="45"/>
+      <c r="C51" s="73"/>
       <c r="D51" s="24"/>
     </row>
     <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="69"/>
+      <c r="B52" s="39"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="41"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="70"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="40"/>
+      <c r="B53" s="42"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="44"/>
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="46"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="40"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="44"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="38"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="40"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="44"/>
     </row>
     <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="71"/>
-      <c r="D56" s="72"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="49"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="60"/>
-      <c r="C57" s="71"/>
-      <c r="D57" s="72"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="49"/>
     </row>
     <row r="58" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="38"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="40"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="44"/>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="40"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="44"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="40"/>
+      <c r="B60" s="46"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="44"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="52"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="40"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="44"/>
     </row>
     <row r="62" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="44"/>
+      <c r="B62" s="64"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="72"/>
     </row>
     <row r="63" spans="1:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="65"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="67"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="38"/>
     </row>
     <row r="64" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="B64" s="21"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
+      <c r="A66" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
     </row>
     <row r="67" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="41"/>
+      <c r="B67" s="63"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
+      <c r="A68" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="34"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
     </row>
     <row r="69" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
     </row>
     <row r="70" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="34"/>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
     </row>
     <row r="72" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
+      <c r="A72" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
     </row>
     <row r="74" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
+      <c r="A74" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="34"/>
-      <c r="C74" s="34"/>
-      <c r="D74" s="34"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
     </row>
     <row r="75" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="34" t="s">
+      <c r="A75" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="34"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
     </row>
     <row r="76" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="34" t="s">
+      <c r="A76" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="34"/>
-      <c r="C76" s="34"/>
-      <c r="D76" s="34"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="34" t="s">
+      <c r="A77" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
     </row>
     <row r="78" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="34"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
     </row>
     <row r="79" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="35" t="s">
+      <c r="A79" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="35"/>
-      <c r="C79" s="35"/>
-      <c r="D79" s="35"/>
+      <c r="B79" s="60"/>
+      <c r="C79" s="60"/>
+      <c r="D79" s="60"/>
     </row>
     <row r="80" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="34" t="s">
+      <c r="A80" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="34"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="34"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
     </row>
     <row r="81" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="34" t="s">
+      <c r="A81" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="34"/>
-      <c r="C81" s="34"/>
-      <c r="D81" s="34"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
@@ -1981,10 +1989,10 @@
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="37" t="s">
+      <c r="C83" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="37"/>
+      <c r="D83" s="34"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
@@ -2002,11 +2010,11 @@
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="64" t="str">
+      <c r="C87" s="35" t="str">
         <f>C42</f>
         <v>________________________________________ Дата_______________</v>
       </c>
-      <c r="D87" s="64"/>
+      <c r="D87" s="35"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
@@ -2066,6 +2074,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="C83:D83"/>
     <mergeCell ref="A28:D28"/>
@@ -2082,55 +2139,6 @@
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A76:D76"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A73:D73"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: increase void between pages
</commit_message>
<xml_diff>
--- a/act.xlsx
+++ b/act.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\xistore_repair-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70246C82-E5BF-47E7-B658-3692CD6705B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8FDB77-129A-4349-854D-8F844FBAD0A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,12 +774,108 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -792,9 +888,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -804,104 +897,11 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1339,7 +1339,7 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -1353,27 +1353,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:5" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1397,9 +1397,9 @@
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="33">
         <f ca="1">NOW()</f>
-        <v>44180.947744791665</v>
+        <v>44180.949689583336</v>
       </c>
       <c r="D6" s="27"/>
     </row>
@@ -1417,58 +1417,58 @@
     </row>
     <row r="9" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="50" t="str">
+      <c r="B9" s="56" t="str">
         <f ca="1">"КВИТАНЦИЯ " &amp; DAY(TODAY()) &amp; "/" &amp; MONTH(TODAY()) &amp; "/20"</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
     </row>
     <row r="11" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="56"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="62"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="54"/>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="62"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="54"/>
       <c r="E15" t="s">
         <v>24</v>
       </c>
@@ -1477,41 +1477,41 @@
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="62"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="54"/>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="45"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="67"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
@@ -1519,132 +1519,132 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
     </row>
     <row r="25" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
     </row>
     <row r="26" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
     </row>
     <row r="30" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
     </row>
     <row r="31" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
     </row>
     <row r="32" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
     </row>
     <row r="34" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
     </row>
     <row r="37" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
@@ -1656,10 +1656,10 @@
       <c r="A39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="34"/>
+      <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
@@ -1673,20 +1673,20 @@
       <c r="A42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="70"/>
+      <c r="D42" s="36"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="34"/>
+      <c r="D43" s="37"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
@@ -1722,7 +1722,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
     </row>
@@ -1737,110 +1737,110 @@
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="25">
         <f ca="1">C6</f>
-        <v>44180.947744791665</v>
-      </c>
-      <c r="B51" s="73" t="str">
+        <v>44180.949689583336</v>
+      </c>
+      <c r="B51" s="45" t="str">
         <f ca="1">B9</f>
         <v>КВИТАНЦИЯ 15/12/20</v>
       </c>
-      <c r="C51" s="73"/>
+      <c r="C51" s="45"/>
       <c r="D51" s="24"/>
     </row>
     <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="39"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="41"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="43"/>
-      <c r="D53" s="44"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="45"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="44"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="40"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="46"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="44"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="47"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="49"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="75"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="47"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="49"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="75"/>
     </row>
     <row r="58" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="46"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="44"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="46"/>
-      <c r="C59" s="43"/>
-      <c r="D59" s="44"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="46"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="44"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="59"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="44"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="64"/>
-      <c r="C62" s="71"/>
-      <c r="D62" s="72"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="44"/>
     </row>
     <row r="63" spans="1:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="36"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="38"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="70"/>
     </row>
     <row r="64" spans="1:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
@@ -1852,132 +1852,132 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B66" s="33"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="63" t="s">
+      <c r="A67" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="63"/>
-      <c r="C67" s="63"/>
-      <c r="D67" s="63"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
+      <c r="A68" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="33"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
     </row>
     <row r="69" spans="1:4" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="33" t="s">
+      <c r="A69" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
     </row>
     <row r="70" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
     </row>
     <row r="72" spans="1:4" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
     </row>
     <row r="74" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
     </row>
     <row r="75" spans="1:4" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
     </row>
     <row r="76" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
     </row>
     <row r="77" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
     </row>
     <row r="78" spans="1:4" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
     </row>
     <row r="79" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="60" t="s">
+      <c r="A79" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="60"/>
-      <c r="C79" s="60"/>
-      <c r="D79" s="60"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
     </row>
     <row r="80" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="33" t="s">
+      <c r="A80" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
     </row>
     <row r="81" spans="1:4" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="33" t="s">
+      <c r="A81" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="33"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
@@ -1989,10 +1989,10 @@
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="34" t="s">
+      <c r="C83" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="34"/>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
@@ -2010,11 +2010,11 @@
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="35" t="str">
+      <c r="C87" s="67" t="str">
         <f>C42</f>
         <v>________________________________________ Дата_______________</v>
       </c>
-      <c r="D87" s="35"/>
+      <c r="D87" s="67"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
@@ -2074,31 +2074,30 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
@@ -2115,30 +2114,31 @@
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A70:D70"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A73:D73"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
HOTFIX: change pages margins
</commit_message>
<xml_diff>
--- a/act.xlsx
+++ b/act.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">квитанция!$A$1:$D$94</definedName>
   </definedNames>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -774,9 +774,102 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -789,9 +882,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,100 +891,10 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,15 +927,15 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2257424</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>194364</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>235004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,15 +977,15 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2257424</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>194364</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>235004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1027,15 +1027,15 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2257424</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>194364</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>235004</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1333,8 +1333,8 @@
   </sheetPr>
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1347,27 +1347,27 @@
   <sheetData>
     <row r="1" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+    </row>
+    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="C6" s="33">
         <f ca="1">NOW()</f>
-        <v>44241.660973726852</v>
+        <v>44246.528821527776</v>
       </c>
       <c r="D6" s="27"/>
     </row>
@@ -1411,58 +1411,58 @@
     </row>
     <row r="9" spans="1:5" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
-      <c r="B9" s="51" t="str">
+      <c r="B9" s="56" t="str">
         <f ca="1">"КВИТАНЦИЯ " &amp; DAY(TODAY()) &amp; "/" &amp; MONTH(TODAY()) &amp; "/20"</f>
-        <v>КВИТАНЦИЯ 14/2/20</v>
-      </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
+        <v>КВИТАНЦИЯ 19/2/20</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
     </row>
     <row r="10" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
     </row>
     <row r="11" spans="1:5" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="55"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="56"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="57"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="62"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="63"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="54"/>
     </row>
     <row r="15" spans="1:5" s="1" customFormat="1" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="62"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="63"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="54"/>
       <c r="E15" t="s">
         <v>24</v>
       </c>
@@ -1471,41 +1471,41 @@
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="63"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="54"/>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B17" s="46"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="69"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="71"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="29" t="s">
@@ -1521,12 +1521,12 @@
       <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
@@ -1617,12 +1617,12 @@
       <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
     </row>
     <row r="36" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="34" t="s">
@@ -1650,10 +1650,10 @@
       <c r="A39" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="35"/>
+      <c r="D39" s="37"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="11"/>
@@ -1667,20 +1667,20 @@
       <c r="A42" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="72"/>
+      <c r="D42" s="36"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B43" s="13"/>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="35"/>
+      <c r="D43" s="37"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="11"/>
@@ -1716,7 +1716,7 @@
       <c r="C48" s="11"/>
       <c r="D48" s="13"/>
     </row>
-    <row r="49" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
     </row>
@@ -1731,110 +1731,110 @@
     <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="25">
         <f ca="1">C6</f>
-        <v>44241.660973726852</v>
-      </c>
-      <c r="B51" s="75" t="str">
+        <v>44246.528821527776</v>
+      </c>
+      <c r="B51" s="45" t="str">
         <f ca="1">B9</f>
-        <v>КВИТАНЦИЯ 14/2/20</v>
-      </c>
-      <c r="C51" s="75"/>
+        <v>КВИТАНЦИЯ 19/2/20</v>
+      </c>
+      <c r="C51" s="45"/>
       <c r="D51" s="24"/>
     </row>
     <row r="52" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="40"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
     </row>
     <row r="53" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="43"/>
-      <c r="C53" s="44"/>
-      <c r="D53" s="45"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="40"/>
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B54" s="46"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="45"/>
+      <c r="C54" s="39"/>
+      <c r="D54" s="40"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B55" s="47"/>
-      <c r="C55" s="44"/>
-      <c r="D55" s="45"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="50"/>
+      <c r="B56" s="63"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="75"/>
     </row>
     <row r="57" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B57" s="48"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="75"/>
     </row>
     <row r="58" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="45"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="47"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="45"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="44"/>
-      <c r="D60" s="45"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="60"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="45"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B62" s="65"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="74"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="44"/>
     </row>
     <row r="63" spans="1:4" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B63" s="37"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="39"/>
+      <c r="B63" s="68"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="70"/>
     </row>
     <row r="64" spans="1:4" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A64" s="26"/>
@@ -1854,12 +1854,12 @@
       <c r="D66" s="34"/>
     </row>
     <row r="67" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="64" t="s">
+      <c r="A67" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="B67" s="64"/>
-      <c r="C67" s="64"/>
-      <c r="D67" s="64"/>
+      <c r="B67" s="41"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
     </row>
     <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="34" t="s">
@@ -1950,12 +1950,12 @@
       <c r="D78" s="34"/>
     </row>
     <row r="79" spans="1:4" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="61" t="s">
+      <c r="A79" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B79" s="61"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
     </row>
     <row r="80" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
@@ -1983,10 +1983,10 @@
       <c r="A83" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D83" s="35"/>
+      <c r="D83" s="37"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
@@ -2004,11 +2004,11 @@
       <c r="A87" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C87" s="36" t="str">
+      <c r="C87" s="67" t="str">
         <f>C42</f>
         <v>________________________________________ Дата_______________</v>
       </c>
-      <c r="D87" s="36"/>
+      <c r="D87" s="67"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
@@ -2068,31 +2068,30 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A74:D74"/>
     <mergeCell ref="A75:D75"/>
@@ -2109,30 +2108,31 @@
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="A70:D70"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A73:D73"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>